<commit_message>
Updated summary statistics, 1275 graph
</commit_message>
<xml_diff>
--- a/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
+++ b/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
@@ -11,18 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Parameters:</t>
   </si>
   <si>
-    <t>% error for no blowouts</t>
-  </si>
-  <si>
-    <t>% error for blowouts</t>
-  </si>
-  <si>
-    <t>%error difference between blowouts and no blowouts</t>
+    <t>% error (blowouts before)</t>
   </si>
   <si>
     <t>Viscosity standard:</t>
@@ -38,14 +32,31 @@
   </si>
   <si>
     <t>Delay dispense:</t>
+  </si>
+  <si>
+    <t>Time for 1000ul</t>
+  </si>
+  <si>
+    <t>1000(ul)</t>
+  </si>
+  <si>
+    <t>500(ul)</t>
+  </si>
+  <si>
+    <t>300(ul)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -105,7 +116,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -323,7 +336,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.5"/>
-    <col customWidth="1" min="14" max="14" width="14.25"/>
+    <col customWidth="1" min="15" max="15" width="14.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -333,69 +346,48 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
-        <v>1000.0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>500.0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1000.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>500.0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1000.0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>500.0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>300.0</v>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>505.0</v>
+        <v>204.0</v>
       </c>
       <c r="B4" s="2">
-        <v>20.0</v>
+        <v>185.0</v>
       </c>
       <c r="C4" s="2">
-        <v>5.0</v>
+        <v>18.0</v>
       </c>
       <c r="D4" s="1">
         <v>10.0</v>
@@ -404,89 +396,145 @@
         <v>10.0</v>
       </c>
       <c r="F4" s="1">
-        <v>-1.813014</v>
+        <v>80.960961</v>
       </c>
       <c r="G4" s="1">
-        <v>-1.027653</v>
+        <v>-0.992463</v>
       </c>
       <c r="H4" s="1">
-        <v>-3.4352</v>
+        <v>-0.665249</v>
       </c>
       <c r="I4" s="1">
-        <v>-2.215764</v>
-      </c>
-      <c r="J4" s="1">
-        <v>-1.799589</v>
-      </c>
-      <c r="K4" s="3">
-        <v>-4.330199</v>
-      </c>
-      <c r="L4" s="4">
-        <f t="shared" ref="L4:N4" si="1">MINUS(F4,I4)</f>
-        <v>0.40275</v>
-      </c>
-      <c r="M4" s="5">
-        <f t="shared" si="1"/>
-        <v>0.771936</v>
-      </c>
-      <c r="N4" s="5">
-        <f t="shared" si="1"/>
-        <v>0.894999</v>
-      </c>
+        <v>-3.022089</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1">
+        <v>398.0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>80.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>99.166667</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-1.767441</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-1.275127</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-3.49754</v>
+      </c>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>505.0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-2.215764</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-1.799589</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-4.330199</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
         <v>817.0</v>
       </c>
-      <c r="B5" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B7" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="C7" s="2">
         <v>5.0</v>
       </c>
-      <c r="D5" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>-2.834948</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-1.798824</v>
-      </c>
-      <c r="H5" s="1">
-        <v>-3.851567</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="D7" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>320.0</v>
+      </c>
+      <c r="G7" s="1">
         <v>-2.759218</v>
       </c>
-      <c r="J5" s="1">
+      <c r="H7" s="1">
         <v>-3.829765</v>
       </c>
-      <c r="K5" s="3">
+      <c r="I7" s="3">
         <v>-4.086789</v>
       </c>
-      <c r="L5" s="1">
-        <f t="shared" ref="L5:N5" si="2">MINUS(F5,I5)</f>
-        <v>-0.07573</v>
-      </c>
-      <c r="M5" s="5">
-        <f t="shared" si="2"/>
-        <v>2.030941</v>
-      </c>
-      <c r="N5" s="5">
-        <f t="shared" si="2"/>
-        <v>0.235222</v>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>1275.0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>670.0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>-2.46707797254956</v>
+      </c>
+      <c r="H8" s="5">
+        <v>-3.7964279316069</v>
+      </c>
+      <c r="I8" s="5">
+        <v>-2.44205883906668</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="D9" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated summary statistics pptx and xlsx
</commit_message>
<xml_diff>
--- a/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
+++ b/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
@@ -445,7 +445,7 @@
         <v>505.0</v>
       </c>
       <c r="B6" s="2">
-        <v>20.0</v>
+        <v>50.0</v>
       </c>
       <c r="C6" s="2">
         <v>5.0</v>
@@ -456,14 +456,17 @@
       <c r="E6" s="1">
         <v>10.0</v>
       </c>
+      <c r="F6" s="5">
+        <v>240.0</v>
+      </c>
       <c r="G6" s="1">
-        <v>-2.215764</v>
+        <v>-1.031009</v>
       </c>
       <c r="H6" s="1">
-        <v>-1.799589</v>
+        <v>-1.581433</v>
       </c>
       <c r="I6" s="3">
-        <v>-4.330199</v>
+        <v>-3.491137</v>
       </c>
     </row>
     <row r="7">
@@ -531,10 +534,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
505 exp3, 817 attempt at exp3 and updated summary stats
</commit_message>
<xml_diff>
--- a/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
+++ b/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
@@ -6,6 +6,9 @@
     <sheet state="visible" name="Manual calibration (sum)" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Manual calibration (indiv)" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="BOTorch (sum)" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="BOTorch (indiv)" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="IPOPT (sum)" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="IPOPT (indiv)" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="19">
   <si>
     <t>Parameters:</t>
   </si>
@@ -62,6 +65,15 @@
   </si>
   <si>
     <t>% error(blowouts before)</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>IPOPT Experiment 2</t>
+  </si>
+  <si>
+    <t>IPOPT Experiment 3</t>
   </si>
 </sst>
 </file>
@@ -178,6 +190,18 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1151,6 +1175,9 @@
       <c r="R3" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="9">
@@ -1181,14 +1208,33 @@
       <c r="J4" s="9">
         <v>204.0</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
+      <c r="K4" s="10">
+        <v>102.939013</v>
+      </c>
+      <c r="L4" s="10">
+        <v>15.379469</v>
+      </c>
+      <c r="M4" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N4" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O4" s="10">
+        <v>94.736242</v>
+      </c>
+      <c r="P4" s="10">
+        <v>-1.985911</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>-0.948609</v>
+      </c>
+      <c r="R4" s="10">
+        <v>-2.128154</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-1.687558</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="10">
@@ -1216,14 +1262,33 @@
       <c r="J5" s="11">
         <v>505.0</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
+      <c r="K5" s="10">
+        <v>43.183051</v>
+      </c>
+      <c r="L5" s="10">
+        <v>7.278616</v>
+      </c>
+      <c r="M5" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N5" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O5" s="10">
+        <v>180.545995</v>
+      </c>
+      <c r="P5" s="10">
+        <v>-1.618352</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>-1.779452</v>
+      </c>
+      <c r="R5" s="10">
+        <v>-1.975233</v>
+      </c>
+      <c r="S5" s="1">
+        <v>-1.791012</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="10">
@@ -1251,14 +1316,33 @@
       <c r="J6" s="11">
         <v>817.0</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
+      <c r="K6" s="10">
+        <v>6.699781</v>
+      </c>
+      <c r="L6" s="10">
+        <v>10.184027</v>
+      </c>
+      <c r="M6" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N6" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>267.451605</v>
+      </c>
+      <c r="P6" s="10">
+        <v>-1.511394</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>-2.982966</v>
+      </c>
+      <c r="R6" s="10">
+        <v>-4.167108</v>
+      </c>
+      <c r="S6" s="1">
+        <v>-2.887156</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="10">
@@ -1286,14 +1370,33 @@
       <c r="J7" s="11">
         <v>1275.0</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
+      <c r="K7" s="10">
+        <v>4.095164</v>
+      </c>
+      <c r="L7" s="10">
+        <v>6.424205</v>
+      </c>
+      <c r="M7" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>419.851735</v>
+      </c>
+      <c r="P7" s="10">
+        <v>-2.824018</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>-3.963222</v>
+      </c>
+      <c r="R7" s="10">
+        <v>-5.928058</v>
+      </c>
+      <c r="S7" s="1">
+        <v>-4.238433</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="12">
@@ -1535,13 +1638,1071 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="J1:R1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="P2:R2"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="J1:S1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.13"/>
+    <col customWidth="1" min="8" max="8" width="19.75"/>
+    <col customWidth="1" min="10" max="10" width="15.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9">
+        <v>204.0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>300.0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>114.512228</v>
+      </c>
+      <c r="D4" s="10">
+        <v>21.217443</v>
+      </c>
+      <c r="E4" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>75.863723</v>
+      </c>
+      <c r="H4" s="10">
+        <v>-2.516088</v>
+      </c>
+      <c r="J4" s="9">
+        <v>204.0</v>
+      </c>
+      <c r="K4" s="10">
+        <v>102.939013</v>
+      </c>
+      <c r="L4" s="10">
+        <v>15.379469</v>
+      </c>
+      <c r="M4" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N4" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O4" s="10">
+        <v>94.736242</v>
+      </c>
+      <c r="P4" s="10">
+        <v>-1.985911</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>-0.948609</v>
+      </c>
+      <c r="R4" s="10">
+        <v>-2.128154</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-1.687558</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="10">
+        <v>300.0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>81.16671</v>
+      </c>
+      <c r="D5" s="10">
+        <v>13.787268</v>
+      </c>
+      <c r="E5" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>104.851008</v>
+      </c>
+      <c r="H5" s="10">
+        <v>-1.138641</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="10">
+        <v>500.0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>75.041981</v>
+      </c>
+      <c r="D6" s="10">
+        <v>18.239168</v>
+      </c>
+      <c r="E6" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>88.152937</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-0.472968</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="10">
+        <v>1000.0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>72.83177</v>
+      </c>
+      <c r="D7" s="10">
+        <v>15.894114</v>
+      </c>
+      <c r="E7" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>96.646646</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-2.098918</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="J8" s="11">
+        <v>505.0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>43.183051</v>
+      </c>
+      <c r="L8" s="10">
+        <v>7.278616</v>
+      </c>
+      <c r="M8" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>180.545995</v>
+      </c>
+      <c r="P8" s="10">
+        <v>-1.618352</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>-1.779452</v>
+      </c>
+      <c r="R8" s="10">
+        <v>-1.975233</v>
+      </c>
+      <c r="S8" s="1">
+        <v>-1.791012</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="12">
+        <v>505.0</v>
+      </c>
+      <c r="B11" s="12">
+        <v>300.0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>44.717819</v>
+      </c>
+      <c r="D11" s="10">
+        <v>9.656528</v>
+      </c>
+      <c r="E11" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G11" s="10">
+        <v>145.91934</v>
+      </c>
+      <c r="H11" s="10">
+        <v>-0.464922</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="12">
+        <v>500.0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>57.178353</v>
+      </c>
+      <c r="D12" s="1">
+        <v>9.26094</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>145.469537</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-1.708971</v>
+      </c>
+      <c r="J12" s="11">
+        <v>817.0</v>
+      </c>
+      <c r="K12" s="10">
+        <v>6.699781</v>
+      </c>
+      <c r="L12" s="10">
+        <v>10.184027</v>
+      </c>
+      <c r="M12" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N12" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O12" s="10">
+        <v>267.451605</v>
+      </c>
+      <c r="P12" s="10">
+        <v>-1.511394</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>-2.982966</v>
+      </c>
+      <c r="R12" s="10">
+        <v>-4.167108</v>
+      </c>
+      <c r="S12" s="1">
+        <v>-2.887156</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="12">
+        <v>1000.0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>76.261096</v>
+      </c>
+      <c r="D13" s="10">
+        <v>16.650269</v>
+      </c>
+      <c r="E13" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>93.171934</v>
+      </c>
+      <c r="H13" s="10">
+        <v>-1.468999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="J15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="11">
+        <v>1275.0</v>
+      </c>
+      <c r="K16" s="10">
+        <v>4.095164</v>
+      </c>
+      <c r="L16" s="10">
+        <v>6.424205</v>
+      </c>
+      <c r="M16" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="N16" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="O16" s="10">
+        <v>419.851735</v>
+      </c>
+      <c r="P16" s="10">
+        <v>-2.824018</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>-3.963222</v>
+      </c>
+      <c r="R16" s="10">
+        <v>-5.928058</v>
+      </c>
+      <c r="S16" s="1">
+        <v>-4.238433</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9">
+        <v>817.0</v>
+      </c>
+      <c r="B17" s="12">
+        <v>300.0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>18.027723</v>
+      </c>
+      <c r="D17" s="10">
+        <v>8.830124</v>
+      </c>
+      <c r="E17" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>188.718812</v>
+      </c>
+      <c r="H17" s="13">
+        <v>-3.56471</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="12">
+        <v>500.0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>16.438385</v>
+      </c>
+      <c r="D18" s="10">
+        <v>7.963184</v>
+      </c>
+      <c r="E18" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>206.411129</v>
+      </c>
+      <c r="H18" s="10">
+        <v>-1.56475</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="12">
+        <v>1000.0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>15.946734</v>
+      </c>
+      <c r="D19" s="10">
+        <v>13.577798</v>
+      </c>
+      <c r="E19" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G19" s="10">
+        <v>156.35841</v>
+      </c>
+      <c r="H19" s="10">
+        <v>-2.210176</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12">
+        <v>1275.0</v>
+      </c>
+      <c r="B23" s="12">
+        <v>300.0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3.867115</v>
+      </c>
+      <c r="D23" s="10">
+        <v>4.755213</v>
+      </c>
+      <c r="E23" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G23" s="10">
+        <v>488.886211</v>
+      </c>
+      <c r="H23" s="10">
+        <v>-7.390287</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="12">
+        <v>500.0</v>
+      </c>
+      <c r="C24" s="10">
+        <v>6.522269</v>
+      </c>
+      <c r="D24" s="10">
+        <v>5.229181</v>
+      </c>
+      <c r="E24" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G24" s="10">
+        <v>364.555419</v>
+      </c>
+      <c r="H24" s="10">
+        <v>-3.853138</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="9">
+        <v>1000.0</v>
+      </c>
+      <c r="C25" s="10">
+        <v>10.888369</v>
+      </c>
+      <c r="D25" s="10">
+        <v>8.013913</v>
+      </c>
+      <c r="E25" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="G25" s="10">
+        <v>236.624113</v>
+      </c>
+      <c r="H25" s="10">
+        <v>-4.110001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="P6:S6"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.0"/>
+    <col customWidth="1" min="8" max="8" width="19.88"/>
+    <col customWidth="1" min="10" max="10" width="14.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="6"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>204.0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>300.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>158.913469</v>
+      </c>
+      <c r="D4" s="1">
+        <v>27.765223</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>62.309012</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-2.937756</v>
+      </c>
+      <c r="J4" s="1">
+        <v>204.0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>158.913469</v>
+      </c>
+      <c r="L4" s="1">
+        <v>27.239269</v>
+      </c>
+      <c r="M4" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>63.004438</v>
+      </c>
+      <c r="P4" s="1">
+        <v>-1.780138</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>-0.715849</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-2.206865</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-1.567617</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="12">
+        <v>500.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>158.913469</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43.4914</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>49.285784</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-0.513448</v>
+      </c>
+      <c r="J5" s="1">
+        <v>505.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="12">
+        <v>1000.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>158.913469</v>
+      </c>
+      <c r="D6" s="1">
+        <v>27.104122</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>63.18749</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-1.30787</v>
+      </c>
+      <c r="J6" s="1">
+        <v>817.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12">
+        <v>505.0</v>
+      </c>
+      <c r="B7" s="12">
+        <v>300.0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1275.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="12">
+        <v>500.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="12">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9">
+        <v>817.0</v>
+      </c>
+      <c r="B10" s="12">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="12">
+        <v>500.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="12">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12">
+        <v>1275.0</v>
+      </c>
+      <c r="B13" s="12">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="12">
+        <v>500.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="12">
+        <v>1000.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="J1:S1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A13:A15"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated graphs and graph code + updated summary stats
</commit_message>
<xml_diff>
--- a/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
+++ b/Sartorious_experiments/Finalised_Data/Viscosity standards best parameters.xlsx
@@ -458,10 +458,10 @@
         <v>204.0</v>
       </c>
       <c r="B4" s="2">
-        <v>185.0</v>
+        <v>150.0</v>
       </c>
       <c r="C4" s="2">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="D4" s="1">
         <v>10.0</v>
@@ -470,16 +470,16 @@
         <v>10.0</v>
       </c>
       <c r="F4" s="1">
-        <v>80.960961</v>
+        <v>93.333333</v>
       </c>
       <c r="G4" s="1">
-        <v>-0.992463</v>
+        <v>-0.383575</v>
       </c>
       <c r="H4" s="1">
-        <v>-0.665249</v>
+        <v>-1.518704</v>
       </c>
       <c r="I4" s="1">
-        <v>-3.022089</v>
+        <v>-2.589177</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="4"/>
@@ -774,10 +774,10 @@
         <v>204.0</v>
       </c>
       <c r="B4" s="2">
-        <v>185.0</v>
+        <v>150.0</v>
       </c>
       <c r="C4" s="2">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="D4" s="1">
         <v>10.0</v>
@@ -786,16 +786,16 @@
         <v>10.0</v>
       </c>
       <c r="F4" s="1">
-        <v>80.960961</v>
+        <v>93.333333</v>
       </c>
       <c r="G4" s="1">
-        <v>-0.992463</v>
+        <v>-0.383575</v>
       </c>
       <c r="H4" s="1">
-        <v>-0.665249</v>
+        <v>-1.518704</v>
       </c>
       <c r="I4" s="1">
-        <v>-3.022089</v>
+        <v>-2.589177</v>
       </c>
     </row>
     <row r="6">
@@ -1317,10 +1317,10 @@
         <v>817.0</v>
       </c>
       <c r="K6" s="10">
-        <v>6.699781</v>
+        <v>16.438385</v>
       </c>
       <c r="L6" s="10">
-        <v>10.184027</v>
+        <v>7.963184</v>
       </c>
       <c r="M6" s="10">
         <v>10.0</v>
@@ -1329,19 +1329,19 @@
         <v>10.0</v>
       </c>
       <c r="O6" s="10">
-        <v>267.451605</v>
+        <v>206.411129</v>
       </c>
       <c r="P6" s="10">
-        <v>-1.511394</v>
+        <v>-0.573375</v>
       </c>
       <c r="Q6" s="10">
-        <v>-2.982966</v>
+        <v>-2.046668</v>
       </c>
       <c r="R6" s="10">
-        <v>-4.167108</v>
+        <v>-3.174586</v>
       </c>
       <c r="S6" s="1">
-        <v>-2.887156</v>
+        <v>-1.931543</v>
       </c>
     </row>
     <row r="7">
@@ -1638,12 +1638,12 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="J1:S1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="K2:O2"/>
+    <mergeCell ref="P2:S2"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="J1:S1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2060,10 +2060,10 @@
         <v>817.0</v>
       </c>
       <c r="K12" s="10">
-        <v>6.699781</v>
+        <v>16.438385</v>
       </c>
       <c r="L12" s="10">
-        <v>10.184027</v>
+        <v>7.963184</v>
       </c>
       <c r="M12" s="10">
         <v>10.0</v>
@@ -2072,19 +2072,19 @@
         <v>10.0</v>
       </c>
       <c r="O12" s="10">
-        <v>267.451605</v>
+        <v>206.411129</v>
       </c>
       <c r="P12" s="10">
-        <v>-1.511394</v>
+        <v>-0.573375</v>
       </c>
       <c r="Q12" s="10">
-        <v>-2.982966</v>
+        <v>-2.046668</v>
       </c>
       <c r="R12" s="10">
-        <v>-4.167108</v>
+        <v>-3.174586</v>
       </c>
       <c r="S12" s="1">
-        <v>-2.887156</v>
+        <v>-1.931543</v>
       </c>
     </row>
     <row r="13">
@@ -2393,22 +2393,22 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C2:G2"/>
     <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="C21:G21"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="K10:O10"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="K14:O14"/>
     <mergeCell ref="P14:S14"/>
-    <mergeCell ref="C2:G2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="K6:O6"/>
     <mergeCell ref="P6:S6"/>
   </mergeCells>
@@ -2680,14 +2680,14 @@
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="J1:S1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="P2:S2"/>
-    <mergeCell ref="J1:S1"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>